<commit_message>
feat(gameloop): Init GameRunning use case for world creation
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_2.xlsx
+++ b/docs/boards/sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2399F230-428C-415C-B83E-29F1CE7B5F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C725747-2DC3-4AC4-8600-28FDA26FC45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2595,16 +2595,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>619183</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>700825</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>403493</xdr:rowOff>
+      <xdr:rowOff>349065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3509256</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3590898</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1945821</xdr:rowOff>
+      <xdr:rowOff>1891393</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2619,7 +2619,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5109540" y="4091029"/>
+          <a:off x="9436611" y="4036601"/>
           <a:ext cx="2890073" cy="1542328"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -4044,16 +4044,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2837148</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2918790</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1274350</xdr:rowOff>
+      <xdr:rowOff>1219922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3357848</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3439490</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1822990</xdr:rowOff>
+      <xdr:rowOff>1768562</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4068,7 +4068,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7327505" y="4961886"/>
+          <a:off x="11654576" y="4907458"/>
           <a:ext cx="520700" cy="548640"/>
         </a:xfrm>
         <a:custGeom>
@@ -5246,8 +5246,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="56" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="56" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat(world): Impl floor generation entirely
</commit_message>
<xml_diff>
--- a/docs/boards/sprint_2.xlsx
+++ b/docs/boards/sprint_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farin\OneDrive\Desktop\Uni\LM_PrimoAnno_1\PPS\PPS-24-Scalata\docs\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C725747-2DC3-4AC4-8600-28FDA26FC45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735614F4-612A-4A4D-9C0F-D0CD93675929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2170,16 +2170,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>621473</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2340687</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2082152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>3511546</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>649015</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>390480</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2194,7 +2194,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5111830" y="6028223"/>
+          <a:off x="17848116" y="8627188"/>
           <a:ext cx="2890073" cy="1165828"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -2386,16 +2386,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>624733</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>583911</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>228636</xdr:rowOff>
+      <xdr:rowOff>2718743</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3514806</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1501145</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3473984</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1133752</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2410,7 +2410,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5115090" y="6773672"/>
+          <a:off x="17810554" y="9263779"/>
           <a:ext cx="2890073" cy="1272509"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -2595,16 +2595,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>700825</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>349065</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>564753</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3590898</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1891393</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3454826</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1619250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2619,7 +2619,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9436611" y="4036601"/>
+          <a:off x="17791396" y="6621958"/>
           <a:ext cx="2890073" cy="1542328"/>
         </a:xfrm>
         <a:prstGeom prst="snip1Rect">
@@ -3739,16 +3739,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2638590</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>759314</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2584161</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>459957</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>3159290</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1307954</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3104861</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1008597</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3763,7 +3763,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7128947" y="7304350"/>
+          <a:off x="19810804" y="9862493"/>
           <a:ext cx="520700" cy="548640"/>
         </a:xfrm>
         <a:custGeom>
@@ -4044,16 +4044,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2918790</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1219922</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2660254</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>961386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>3439490</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1768562</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3180954</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1510026</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4068,7 +4068,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11654576" y="4907458"/>
+          <a:off x="19886897" y="7506422"/>
           <a:ext cx="520700" cy="548640"/>
         </a:xfrm>
         <a:custGeom>
@@ -5246,8 +5246,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="56" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="56" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5303,7 +5303,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="27">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>14</v>

</xml_diff>